<commit_message>
Mise en forme pour édition au format poker.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -55,8 +55,8 @@
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">HIPPo : C’est le chef (la personne la plus importante, la mieux payée, la plus forte...) qui décide pour tout le monde. 
-Variantes : 
+    <t xml:space="preserve">HIPPo : C’est le chef (la personne la plus importante, la mieux payée, la plus forte…) qui décide pour tout le monde.
+&lt;u&gt;Variantes :&lt;/u&gt;
 Oligarchie (les plus âgés décident). 
 Vote féminin/masculin (seul.e.s les filles/garçons décident). </t>
   </si>
@@ -107,7 +107,7 @@
  - Je suis d’accord : &lt;b&gt;pouce levé&lt;/b&gt;
  - Je consens : &lt;b&gt;main horizontale ou à plat&lt;/b&gt;. En consentant, j’exprime une opinion. Je consens que la personne ayant proposé aille plus loin.
  - Je mets mon veto : &lt;b&gt;pouce en bas&lt;/b&gt;. Si je mets un veto, je dois expliquer les raisons de mon veto et proposer une porte de sortie. Je serais d’accord si… 
-Pour que la décision soit prise, il ne faut aucun veto et une majorité de ‘Pour’.</t>
+Pour que la décision soit prise, il ne faut aucun veto et majorité de ‘Pour’.</t>
   </si>
   <si>
     <t xml:space="preserve">Conseil</t>
@@ -134,10 +134,10 @@
     <t xml:space="preserve">Choix commun</t>
   </si>
   <si>
-    <t xml:space="preserve">Chaque votant donne à chacune des propositions une mention compréhensible par tous : Excellent/Très bien/Bien/Assez bien/Passable/Insuffisant/À rejeter. 
-En prenant en compte l’ensemble des votes, cela donne à chaque proposition, un profil. 
-La proposition, qui a le meilleur profil est choisi : c’est celui qui aura les mentions les plus favorables. 
-Et si aucun.e proposition, n’a de profil très favorable, on peut rediscuter des propositions !</t>
+    <t xml:space="preserve">Chaque votant donne à chacune des propositions une mention claire pour tous : Excellent/Très bien/Bien/Assez bien/Passable/Insuffisant/À rejeter. 
+En prenant en compte l’ensemble des votes, cela donne à chaque proposition un profil. 
+La proposition, qui a le meilleur profil est choisie : c’est celui qui aura les mentions les plus favorables. 
+Si aucune proposition n’a de profil très favorable, on peut rediscuter celles-ci !</t>
   </si>
   <si>
     <t xml:space="preserve">Bac à sable</t>
@@ -176,12 +176,13 @@
     <t xml:space="preserve">table</t>
   </si>
   <si>
-    <t xml:space="preserve">Une ou plusieurs questions-problématiques sont inscrites sur &lt;b&gt;chaque coin d’une nappe&lt;/b&gt;.
+    <t xml:space="preserve">Une ou plusieurs problématiques sont inscrites sur &lt;b&gt;chaque coin d’une nappe&lt;/b&gt;.
 Les participants doivent répondre, en 3-5 min, à la question &lt;b&gt;devant eux&lt;/b&gt;.
 A la fin du temps imparti, &lt;b&gt;la nappe tourne&lt;/b&gt; devant les participants. Et on recommence.
-Astuces :
+&lt;u&gt;Astuces :&lt;/u&gt;
 Faire autant de tours que de participants. Chacun pourra ainsi enrichir chaque sujet.
-Augmenter le temps imparti si les participants n’ont pas le temps de tout lire.</t>
+Augmenter le temps imparti si les participants n’ont pas le temps de 
+tout lire.</t>
   </si>
   <si>
     <t xml:space="preserve">World Café</t>
@@ -203,7 +204,7 @@
   </si>
   <si>
     <t xml:space="preserve">Au centre de la feuille/tableau, Écrire &lt;b&gt;un&lt;/b&gt; mot/une phrase qui résume la problématique.
-Raccrocher les mots/concepts qui &lt;b&gt;gravitent&lt;/b&gt; autour, les mettre sous forme d'ilôt.
+Raccrocher les mots/concepts qui &lt;b&gt;gravitent&lt;/b&gt; autour, les mettre sous forme d'ilôts.
 Enrichir les concepts représentés.</t>
   </si>
   <si>
@@ -231,7 +232,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -252,6 +253,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -296,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -307,6 +314,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -326,10 +337,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -363,7 +374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="79.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -434,7 +445,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="98.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -450,6 +461,7 @@
       <c r="F6" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -468,7 +480,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -485,7 +497,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="89.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -539,7 +551,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="69.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="118.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -573,7 +585,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="30.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
@@ -591,17 +603,15 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="0"/>
       <c r="F15" s="2" t="s">
         <v>52</v>
       </c>
@@ -655,8 +665,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"DejaVu Serif,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"DejaVu Serif,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"DejaVu Serif,Book"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"DejaVu Serif,Book"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>